<commit_message>
last minor changes to report
</commit_message>
<xml_diff>
--- a/excel/expected.xlsx
+++ b/excel/expected.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14260" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
@@ -516,11 +516,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2101739880"/>
-        <c:axId val="2101736952"/>
+        <c:axId val="2065018744"/>
+        <c:axId val="2065021432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2101739880"/>
+        <c:axId val="2065018744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -530,7 +530,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2101736952"/>
+        <c:crossAx val="2065021432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -538,7 +538,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2101736952"/>
+        <c:axId val="2065021432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -549,7 +549,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2101739880"/>
+        <c:crossAx val="2065018744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -928,10 +928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AZ38"/>
+  <dimension ref="A1:AZ37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="A38" sqref="A38:AZ38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1954,213 +1954,57 @@
       </c>
     </row>
     <row r="8" spans="1:52">
-      <c r="A8">
-        <v>41</v>
-      </c>
-      <c r="B8" s="1">
-        <f t="shared" si="2"/>
-        <v>999.96889649239029</v>
-      </c>
-      <c r="C8" s="1">
-        <f t="shared" si="2"/>
-        <v>2905.5449088977784</v>
-      </c>
-      <c r="D8" s="1">
-        <f t="shared" si="0"/>
-        <v>4372.0969950952194</v>
-      </c>
-      <c r="E8" s="1">
-        <f t="shared" si="0"/>
-        <v>5409.6610825001871</v>
-      </c>
-      <c r="F8" s="1">
-        <f t="shared" si="0"/>
-        <v>6157.7244362720985</v>
-      </c>
-      <c r="G8" s="1">
-        <f t="shared" si="0"/>
-        <v>6716.1488493726283</v>
-      </c>
-      <c r="H8" s="1">
-        <f t="shared" si="0"/>
-        <v>7146.7586213636205</v>
-      </c>
-      <c r="I8" s="1">
-        <f t="shared" si="0"/>
-        <v>7488.0595419218307</v>
-      </c>
-      <c r="J8" s="1">
-        <f t="shared" si="0"/>
-        <v>7764.8308802453375</v>
-      </c>
-      <c r="K8" s="1">
-        <f t="shared" si="0"/>
-        <v>7993.5964623787249</v>
-      </c>
-      <c r="L8" s="1">
-        <f t="shared" si="0"/>
-        <v>8185.7440709896</v>
-      </c>
-      <c r="M8" s="1">
-        <f t="shared" si="0"/>
-        <v>8349.3542748000782</v>
-      </c>
-      <c r="N8" s="1">
-        <f t="shared" si="0"/>
-        <v>8490.3092572325622</v>
-      </c>
-      <c r="O8" s="1">
-        <f t="shared" si="0"/>
-        <v>8612.9876268057906</v>
-      </c>
-      <c r="P8" s="1">
-        <f t="shared" si="0"/>
-        <v>8720.7132576529057</v>
-      </c>
-      <c r="Q8" s="1">
-        <f t="shared" si="0"/>
-        <v>8816.0533336579228</v>
-      </c>
-      <c r="R8" s="1">
-        <f t="shared" si="0"/>
-        <v>8901.0212179361533</v>
-      </c>
-      <c r="S8" s="1">
-        <f t="shared" si="0"/>
-        <v>8977.2176399498185</v>
-      </c>
-      <c r="T8" s="1">
-        <f t="shared" si="0"/>
-        <v>9045.9309359314557</v>
-      </c>
-      <c r="U8" s="1">
-        <f t="shared" si="0"/>
-        <v>9108.2095092748514</v>
-      </c>
-      <c r="V8" s="1">
-        <f t="shared" si="1"/>
-        <v>9164.9150698552785</v>
-      </c>
-      <c r="W8" s="1">
-        <f t="shared" si="1"/>
-        <v>9216.7623324357774</v>
-      </c>
-      <c r="X8" s="1">
-        <f t="shared" si="1"/>
-        <v>9264.349019773701</v>
-      </c>
-      <c r="Y8" s="1">
-        <f t="shared" si="1"/>
-        <v>9308.1788187995171</v>
-      </c>
-      <c r="Z8" s="1">
-        <f t="shared" si="1"/>
-        <v>9348.6791449905104</v>
-      </c>
-      <c r="AA8" s="1">
-        <f t="shared" si="1"/>
-        <v>9386.2150322167054</v>
-      </c>
-      <c r="AB8" s="1">
-        <f t="shared" si="1"/>
-        <v>9421.1000981347825</v>
-      </c>
-      <c r="AC8" s="1">
-        <f t="shared" si="1"/>
-        <v>9453.6052782487677</v>
-      </c>
-      <c r="AD8" s="1">
-        <f t="shared" si="1"/>
-        <v>9483.9658402239802</v>
-      </c>
-      <c r="AE8" s="1">
-        <f t="shared" si="1"/>
-        <v>9512.387060026158</v>
-      </c>
-      <c r="AF8" s="1">
-        <f t="shared" si="1"/>
-        <v>9539.0488493004923</v>
-      </c>
-      <c r="AG8" s="1">
-        <f t="shared" si="1"/>
-        <v>9564.1095518591974</v>
-      </c>
-      <c r="AH8" s="1">
-        <f t="shared" si="1"/>
-        <v>9587.7090791258106</v>
-      </c>
-      <c r="AI8" s="1">
-        <f t="shared" si="1"/>
-        <v>9609.9715140280732</v>
-      </c>
-      <c r="AJ8" s="1">
-        <f t="shared" si="1"/>
-        <v>9631.0072866971659</v>
-      </c>
-      <c r="AK8" s="1">
-        <f t="shared" si="1"/>
-        <v>9650.9150000579393</v>
-      </c>
-      <c r="AL8" s="1">
-        <f t="shared" si="1"/>
-        <v>9669.7829714967411</v>
-      </c>
-      <c r="AM8" s="1">
-        <f t="shared" si="1"/>
-        <v>9687.6905386098133</v>
-      </c>
-      <c r="AN8" s="1">
-        <f t="shared" si="1"/>
-        <v>9704.70917204752</v>
-      </c>
-      <c r="AO8" s="1">
-        <f t="shared" si="1"/>
-        <v>9720.9034260780572</v>
-      </c>
-      <c r="AP8" s="1">
-        <f t="shared" si="1"/>
-        <v>9736.3317551274904</v>
-      </c>
-      <c r="AQ8" s="1">
-        <f t="shared" si="1"/>
-        <v>9751.047217598858</v>
-      </c>
-      <c r="AR8" s="1">
-        <f t="shared" si="1"/>
-        <v>9765.0980837161769</v>
-      </c>
-      <c r="AS8" s="1">
-        <f t="shared" si="1"/>
-        <v>9778.528363819014</v>
-      </c>
-      <c r="AT8" s="1">
-        <f t="shared" si="1"/>
-        <v>9791.3782677349536</v>
-      </c>
-      <c r="AU8" s="1">
-        <f t="shared" si="1"/>
-        <v>9803.6846065801128</v>
-      </c>
-      <c r="AV8" s="1">
-        <f t="shared" si="1"/>
-        <v>9815.4811436775308</v>
-      </c>
-      <c r="AW8" s="1">
-        <f t="shared" si="1"/>
-        <v>9826.7989039102595</v>
-      </c>
-      <c r="AX8" s="1">
-        <f t="shared" si="1"/>
-        <v>9837.6664458273481</v>
-      </c>
-      <c r="AY8" s="1">
-        <f t="shared" si="1"/>
-        <v>9848.1101013096813</v>
-      </c>
-      <c r="AZ8" s="1">
-        <f t="shared" si="1"/>
-        <v>9858.1541890129629</v>
-      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+      <c r="AC8" s="1"/>
+      <c r="AD8" s="1"/>
+      <c r="AE8" s="1"/>
+      <c r="AF8" s="1"/>
+      <c r="AG8" s="1"/>
+      <c r="AH8" s="1"/>
+      <c r="AI8" s="1"/>
+      <c r="AJ8" s="1"/>
+      <c r="AK8" s="1"/>
+      <c r="AL8" s="1"/>
+      <c r="AM8" s="1"/>
+      <c r="AN8" s="1"/>
+      <c r="AO8" s="1"/>
+      <c r="AP8" s="1"/>
+      <c r="AQ8" s="1"/>
+      <c r="AR8" s="1"/>
+      <c r="AS8" s="1"/>
+      <c r="AT8" s="1"/>
+      <c r="AU8" s="1"/>
+      <c r="AV8" s="1"/>
+      <c r="AW8" s="1"/>
+      <c r="AX8" s="1"/>
+      <c r="AY8" s="1"/>
+      <c r="AZ8" s="1"/>
     </row>
     <row r="9" spans="1:52">
       <c r="B9" s="1"/>
@@ -3212,213 +3056,57 @@
       </c>
     </row>
     <row r="18" spans="1:52">
-      <c r="A18">
-        <v>41</v>
-      </c>
-      <c r="B18" s="1">
-        <f t="shared" si="5"/>
-        <v>1000</v>
-      </c>
-      <c r="C18" s="1">
-        <f t="shared" si="3"/>
-        <v>3000</v>
-      </c>
-      <c r="D18" s="1">
-        <f t="shared" si="3"/>
-        <v>5000</v>
-      </c>
-      <c r="E18" s="1">
-        <f t="shared" si="3"/>
-        <v>7000</v>
-      </c>
-      <c r="F18" s="1">
-        <f t="shared" si="3"/>
-        <v>9000</v>
-      </c>
-      <c r="G18" s="1">
-        <f t="shared" si="3"/>
-        <v>11000</v>
-      </c>
-      <c r="H18" s="1">
-        <f t="shared" si="3"/>
-        <v>13000</v>
-      </c>
-      <c r="I18" s="1">
-        <f t="shared" si="3"/>
-        <v>15000</v>
-      </c>
-      <c r="J18" s="1">
-        <f t="shared" si="3"/>
-        <v>17000</v>
-      </c>
-      <c r="K18" s="1">
-        <f t="shared" si="3"/>
-        <v>19000</v>
-      </c>
-      <c r="L18" s="1">
-        <f t="shared" si="3"/>
-        <v>20999.999999999964</v>
-      </c>
-      <c r="M18" s="1">
-        <f t="shared" si="3"/>
-        <v>22999.999999999243</v>
-      </c>
-      <c r="N18" s="1">
-        <f t="shared" si="3"/>
-        <v>24999.999999990156</v>
-      </c>
-      <c r="O18" s="1">
-        <f t="shared" si="3"/>
-        <v>26999.999999911779</v>
-      </c>
-      <c r="P18" s="1">
-        <f t="shared" si="3"/>
-        <v>28999.999999412856</v>
-      </c>
-      <c r="Q18" s="1">
-        <f t="shared" si="3"/>
-        <v>30999.999996926501</v>
-      </c>
-      <c r="R18" s="1">
-        <f t="shared" si="3"/>
-        <v>32999.999986784569</v>
-      </c>
-      <c r="S18" s="1">
-        <f t="shared" si="3"/>
-        <v>34999.999951734237</v>
-      </c>
-      <c r="T18" s="1">
-        <f t="shared" si="3"/>
-        <v>36999.999846283172</v>
-      </c>
-      <c r="U18" s="1">
-        <f t="shared" si="3"/>
-        <v>38999.999564077472</v>
-      </c>
-      <c r="V18" s="1">
-        <f t="shared" si="3"/>
-        <v>40999.998880513354</v>
-      </c>
-      <c r="W18" s="1">
-        <f t="shared" si="4"/>
-        <v>42999.997360567082</v>
-      </c>
-      <c r="X18" s="1">
-        <f t="shared" si="4"/>
-        <v>44999.994221838089</v>
-      </c>
-      <c r="Y18" s="1">
-        <f t="shared" si="4"/>
-        <v>46999.98814421799</v>
-      </c>
-      <c r="Z18" s="1">
-        <f t="shared" si="4"/>
-        <v>48999.9770203113</v>
-      </c>
-      <c r="AA18" s="1">
-        <f t="shared" si="4"/>
-        <v>50999.957644389826</v>
-      </c>
-      <c r="AB18" s="1">
-        <f t="shared" si="4"/>
-        <v>52999.925341778529</v>
-      </c>
-      <c r="AC18" s="1">
-        <f t="shared" si="4"/>
-        <v>54999.873544641028</v>
-      </c>
-      <c r="AD18" s="1">
-        <f t="shared" si="4"/>
-        <v>56999.793323722915</v>
-      </c>
-      <c r="AE18" s="1">
-        <f t="shared" si="4"/>
-        <v>58999.672888409463</v>
-      </c>
-      <c r="AF18" s="1">
-        <f t="shared" si="4"/>
-        <v>60999.497069290548</v>
-      </c>
-      <c r="AG18" s="1">
-        <f t="shared" si="4"/>
-        <v>62999.246798259912</v>
-      </c>
-      <c r="AH18" s="1">
-        <f t="shared" si="4"/>
-        <v>64998.898601075642</v>
-      </c>
-      <c r="AI18" s="1">
-        <f t="shared" si="4"/>
-        <v>66998.424116409442</v>
-      </c>
-      <c r="AJ18" s="1">
-        <f t="shared" si="4"/>
-        <v>68997.78965389567</v>
-      </c>
-      <c r="AK18" s="1">
-        <f t="shared" si="4"/>
-        <v>70996.955801737888</v>
-      </c>
-      <c r="AL18" s="1">
-        <f t="shared" si="4"/>
-        <v>72995.877092240829</v>
-      </c>
-      <c r="AM18" s="1">
-        <f t="shared" si="4"/>
-        <v>74994.501731339595</v>
-      </c>
-      <c r="AN18" s="1">
-        <f t="shared" si="4"/>
-        <v>76992.77139596772</v>
-      </c>
-      <c r="AO18" s="1">
-        <f t="shared" si="4"/>
-        <v>78990.621100990291</v>
-      </c>
-      <c r="AP18" s="1">
-        <f t="shared" si="4"/>
-        <v>80987.979135555826</v>
-      </c>
-      <c r="AQ18" s="1">
-        <f t="shared" si="4"/>
-        <v>82984.767067085457</v>
-      </c>
-      <c r="AR18" s="1">
-        <f t="shared" si="4"/>
-        <v>84980.899809747018</v>
-      </c>
-      <c r="AS18" s="1">
-        <f t="shared" si="4"/>
-        <v>86976.28575321789</v>
-      </c>
-      <c r="AT18" s="1">
-        <f t="shared" si="4"/>
-        <v>88970.82694669436</v>
-      </c>
-      <c r="AU18" s="1">
-        <f t="shared" si="4"/>
-        <v>90964.41933258262</v>
-      </c>
-      <c r="AV18" s="1">
-        <f t="shared" si="4"/>
-        <v>92956.953023903203</v>
-      </c>
-      <c r="AW18" s="1">
-        <f t="shared" si="4"/>
-        <v>94948.312619383403</v>
-      </c>
-      <c r="AX18" s="1">
-        <f t="shared" si="4"/>
-        <v>96938.377550137549</v>
-      </c>
-      <c r="AY18" s="1">
-        <f t="shared" si="4"/>
-        <v>98927.022451980694</v>
-      </c>
-      <c r="AZ18" s="1">
-        <f t="shared" si="4"/>
-        <v>100914.11755778526</v>
-      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="1"/>
+      <c r="AA18" s="1"/>
+      <c r="AB18" s="1"/>
+      <c r="AC18" s="1"/>
+      <c r="AD18" s="1"/>
+      <c r="AE18" s="1"/>
+      <c r="AF18" s="1"/>
+      <c r="AG18" s="1"/>
+      <c r="AH18" s="1"/>
+      <c r="AI18" s="1"/>
+      <c r="AJ18" s="1"/>
+      <c r="AK18" s="1"/>
+      <c r="AL18" s="1"/>
+      <c r="AM18" s="1"/>
+      <c r="AN18" s="1"/>
+      <c r="AO18" s="1"/>
+      <c r="AP18" s="1"/>
+      <c r="AQ18" s="1"/>
+      <c r="AR18" s="1"/>
+      <c r="AS18" s="1"/>
+      <c r="AT18" s="1"/>
+      <c r="AU18" s="1"/>
+      <c r="AV18" s="1"/>
+      <c r="AW18" s="1"/>
+      <c r="AX18" s="1"/>
+      <c r="AY18" s="1"/>
+      <c r="AZ18" s="1"/>
     </row>
     <row r="19" spans="1:52">
       <c r="B19" s="1"/>
@@ -4473,213 +4161,57 @@
       </c>
     </row>
     <row r="28" spans="1:52">
-      <c r="A28">
-        <v>41</v>
-      </c>
-      <c r="B28" s="1">
-        <f t="shared" si="7"/>
-        <v>999.96889649239029</v>
-      </c>
-      <c r="C28" s="1">
-        <f t="shared" si="6"/>
-        <v>2905.5449088977784</v>
-      </c>
-      <c r="D28" s="1">
-        <f t="shared" si="6"/>
-        <v>4372.0969950952194</v>
-      </c>
-      <c r="E28" s="1">
-        <f t="shared" si="6"/>
-        <v>5409.6610825001871</v>
-      </c>
-      <c r="F28" s="1">
-        <f t="shared" si="6"/>
-        <v>6157.7244362720985</v>
-      </c>
-      <c r="G28" s="1">
-        <f t="shared" si="6"/>
-        <v>6716.1488493726283</v>
-      </c>
-      <c r="H28" s="1">
-        <f t="shared" si="6"/>
-        <v>7146.7586213636205</v>
-      </c>
-      <c r="I28" s="1">
-        <f t="shared" si="6"/>
-        <v>7488.0595419218307</v>
-      </c>
-      <c r="J28" s="1">
-        <f t="shared" si="6"/>
-        <v>7764.8308802453375</v>
-      </c>
-      <c r="K28" s="1">
-        <f t="shared" si="6"/>
-        <v>7993.5964623787249</v>
-      </c>
-      <c r="L28" s="1">
-        <f t="shared" si="6"/>
-        <v>8185.7440709895855</v>
-      </c>
-      <c r="M28" s="1">
-        <f t="shared" si="6"/>
-        <v>8349.3542747998035</v>
-      </c>
-      <c r="N28" s="1">
-        <f t="shared" si="6"/>
-        <v>8490.3092572292189</v>
-      </c>
-      <c r="O28" s="1">
-        <f t="shared" si="6"/>
-        <v>8612.987626777649</v>
-      </c>
-      <c r="P28" s="1">
-        <f t="shared" si="6"/>
-        <v>8720.7132574763436</v>
-      </c>
-      <c r="Q28" s="1">
-        <f t="shared" si="6"/>
-        <v>8816.0533327838548</v>
-      </c>
-      <c r="R28" s="1">
-        <f t="shared" si="6"/>
-        <v>8901.0212143715835</v>
-      </c>
-      <c r="S28" s="1">
-        <f t="shared" si="6"/>
-        <v>8977.2176275700403</v>
-      </c>
-      <c r="T28" s="1">
-        <f t="shared" si="6"/>
-        <v>9045.9308983500559</v>
-      </c>
-      <c r="U28" s="1">
-        <f t="shared" si="6"/>
-        <v>9108.2094074678334</v>
-      </c>
-      <c r="V28" s="1">
-        <f t="shared" si="6"/>
-        <v>9164.9148196113747</v>
-      </c>
-      <c r="W28" s="1">
-        <f t="shared" si="6"/>
-        <v>9216.7617666909882</v>
-      </c>
-      <c r="X28" s="1">
-        <f t="shared" si="6"/>
-        <v>9264.347830197954</v>
-      </c>
-      <c r="Y28" s="1">
-        <f t="shared" si="6"/>
-        <v>9308.1764708050705</v>
-      </c>
-      <c r="Z28" s="1">
-        <f t="shared" si="6"/>
-        <v>9348.6747607101734</v>
-      </c>
-      <c r="AA28" s="1">
-        <f t="shared" si="6"/>
-        <v>9386.2072369448433</v>
-      </c>
-      <c r="AB28" s="1">
-        <f t="shared" si="6"/>
-        <v>9421.0868271427535</v>
-      </c>
-      <c r="AC28" s="1">
-        <f t="shared" si="6"/>
-        <v>9453.5835426296926</v>
-      </c>
-      <c r="AD28" s="1">
-        <f t="shared" si="6"/>
-        <v>9483.9314523160519</v>
-      </c>
-      <c r="AE28" s="1">
-        <f t="shared" si="6"/>
-        <v>9512.3343208386832</v>
-      </c>
-      <c r="AF28" s="1">
-        <f t="shared" si="6"/>
-        <v>9538.9702020774566</v>
-      </c>
-      <c r="AG28" s="1">
-        <f t="shared" si="6"/>
-        <v>9563.9952073519453</v>
-      </c>
-      <c r="AH28" s="1">
-        <f t="shared" si="6"/>
-        <v>9587.5466192417043</v>
-      </c>
-      <c r="AI28" s="1">
-        <f t="shared" si="6"/>
-        <v>9609.7454812457636</v>
-      </c>
-      <c r="AJ28" s="1">
-        <f t="shared" si="6"/>
-        <v>9630.6987669951814</v>
-      </c>
-      <c r="AK28" s="1">
-        <f t="shared" si="6"/>
-        <v>9650.501207118914</v>
-      </c>
-      <c r="AL28" s="1">
-        <f t="shared" si="6"/>
-        <v>9669.2368396714992</v>
-      </c>
-      <c r="AM28" s="1">
-        <f t="shared" si="6"/>
-        <v>9686.980331606077</v>
-      </c>
-      <c r="AN28" s="1">
-        <f t="shared" si="6"/>
-        <v>9703.7981136078688</v>
-      </c>
-      <c r="AO28" s="1">
-        <f t="shared" si="6"/>
-        <v>9719.7493580841801</v>
-      </c>
-      <c r="AP28" s="1">
-        <f t="shared" si="6"/>
-        <v>9734.886827668086</v>
-      </c>
-      <c r="AQ28" s="1">
-        <f t="shared" si="6"/>
-        <v>9749.2576146095525</v>
-      </c>
-      <c r="AR28" s="1">
-        <f t="shared" si="6"/>
-        <v>9762.9037868780815</v>
-      </c>
-      <c r="AS28" s="1">
-        <f t="shared" si="6"/>
-        <v>9775.8629565226311</v>
-      </c>
-      <c r="AT28" s="1">
-        <f t="shared" si="6"/>
-        <v>9788.1687800929267</v>
-      </c>
-      <c r="AU28" s="1">
-        <f t="shared" si="6"/>
-        <v>9799.8514017289981</v>
-      </c>
-      <c r="AV28" s="1">
-        <f t="shared" si="6"/>
-        <v>9810.9378449445157</v>
-      </c>
-      <c r="AW28" s="1">
-        <f t="shared" si="6"/>
-        <v>9821.4523618556359</v>
-      </c>
-      <c r="AX28" s="1">
-        <f t="shared" si="6"/>
-        <v>9831.4167436900116</v>
-      </c>
-      <c r="AY28" s="1">
-        <f t="shared" si="6"/>
-        <v>9840.8505969882899</v>
-      </c>
-      <c r="AZ28" s="1">
-        <f t="shared" si="6"/>
-        <v>9849.7715914141318</v>
-      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="1"/>
+      <c r="U28" s="1"/>
+      <c r="V28" s="1"/>
+      <c r="W28" s="1"/>
+      <c r="X28" s="1"/>
+      <c r="Y28" s="1"/>
+      <c r="Z28" s="1"/>
+      <c r="AA28" s="1"/>
+      <c r="AB28" s="1"/>
+      <c r="AC28" s="1"/>
+      <c r="AD28" s="1"/>
+      <c r="AE28" s="1"/>
+      <c r="AF28" s="1"/>
+      <c r="AG28" s="1"/>
+      <c r="AH28" s="1"/>
+      <c r="AI28" s="1"/>
+      <c r="AJ28" s="1"/>
+      <c r="AK28" s="1"/>
+      <c r="AL28" s="1"/>
+      <c r="AM28" s="1"/>
+      <c r="AN28" s="1"/>
+      <c r="AO28" s="1"/>
+      <c r="AP28" s="1"/>
+      <c r="AQ28" s="1"/>
+      <c r="AR28" s="1"/>
+      <c r="AS28" s="1"/>
+      <c r="AT28" s="1"/>
+      <c r="AU28" s="1"/>
+      <c r="AV28" s="1"/>
+      <c r="AW28" s="1"/>
+      <c r="AX28" s="1"/>
+      <c r="AY28" s="1"/>
+      <c r="AZ28" s="1"/>
     </row>
     <row r="29" spans="1:52">
       <c r="B29" s="1"/>
@@ -5733,215 +5265,6 @@
         <v>1.8124055393685813E-31</v>
       </c>
     </row>
-    <row r="38" spans="1:52">
-      <c r="A38">
-        <v>41</v>
-      </c>
-      <c r="B38">
-        <f t="shared" si="9"/>
-        <v>17634.497021490657</v>
-      </c>
-      <c r="C38">
-        <f t="shared" si="8"/>
-        <v>4756.3823838769631</v>
-      </c>
-      <c r="D38">
-        <f t="shared" si="8"/>
-        <v>72.015844235817156</v>
-      </c>
-      <c r="E38">
-        <f t="shared" si="8"/>
-        <v>0.45485149121895463</v>
-      </c>
-      <c r="F38">
-        <f t="shared" si="8"/>
-        <v>3.0846385170982477E-3</v>
-      </c>
-      <c r="G38">
-        <f t="shared" si="8"/>
-        <v>2.8956738912323637E-5</v>
-      </c>
-      <c r="H38">
-        <f t="shared" si="8"/>
-        <v>3.9238568620044315E-7</v>
-      </c>
-      <c r="I38">
-        <f t="shared" si="8"/>
-        <v>7.5217024232941279E-9</v>
-      </c>
-      <c r="J38">
-        <f t="shared" si="8"/>
-        <v>1.9675382639239878E-10</v>
-      </c>
-      <c r="K38">
-        <f t="shared" si="8"/>
-        <v>6.7678434521919797E-12</v>
-      </c>
-      <c r="L38">
-        <f t="shared" si="8"/>
-        <v>2.9601279503080337E-13</v>
-      </c>
-      <c r="M38">
-        <f t="shared" si="8"/>
-        <v>1.5989839194366849E-14</v>
-      </c>
-      <c r="N38">
-        <f t="shared" si="8"/>
-        <v>1.0404960952000016E-15</v>
-      </c>
-      <c r="O38">
-        <f t="shared" si="8"/>
-        <v>7.9856329147396829E-17</v>
-      </c>
-      <c r="P38">
-        <f t="shared" si="8"/>
-        <v>7.0995575501599212E-18</v>
-      </c>
-      <c r="Q38">
-        <f t="shared" si="8"/>
-        <v>7.1999591090243772E-19</v>
-      </c>
-      <c r="R38">
-        <f t="shared" si="8"/>
-        <v>8.2201295652365867E-20</v>
-      </c>
-      <c r="S38">
-        <f t="shared" si="8"/>
-        <v>1.0445734783587411E-20</v>
-      </c>
-      <c r="T38">
-        <f t="shared" si="8"/>
-        <v>1.4629521799702948E-21</v>
-      </c>
-      <c r="U38">
-        <f t="shared" si="8"/>
-        <v>2.2388310114760841E-22</v>
-      </c>
-      <c r="V38">
-        <f t="shared" si="8"/>
-        <v>3.7157333516171591E-23</v>
-      </c>
-      <c r="W38">
-        <f t="shared" si="8"/>
-        <v>6.6438999356862662E-24</v>
-      </c>
-      <c r="X38">
-        <f t="shared" si="8"/>
-        <v>1.2723681697636593E-24</v>
-      </c>
-      <c r="Y38">
-        <f t="shared" si="8"/>
-        <v>2.5962928888835399E-25</v>
-      </c>
-      <c r="Z38">
-        <f t="shared" si="8"/>
-        <v>5.6186208495076251E-26</v>
-      </c>
-      <c r="AA38">
-        <f t="shared" si="8"/>
-        <v>1.2842080396494817E-26</v>
-      </c>
-      <c r="AB38">
-        <f t="shared" si="8"/>
-        <v>3.0884994264452918E-27</v>
-      </c>
-      <c r="AC38">
-        <f t="shared" si="8"/>
-        <v>7.7893599496702776E-28</v>
-      </c>
-      <c r="AD38">
-        <f t="shared" si="8"/>
-        <v>2.0538678379910639E-28</v>
-      </c>
-      <c r="AE38">
-        <f t="shared" si="8"/>
-        <v>5.6461936547191767E-29</v>
-      </c>
-      <c r="AF38">
-        <f t="shared" si="8"/>
-        <v>1.6141907681363826E-29</v>
-      </c>
-      <c r="AG38">
-        <f t="shared" si="8"/>
-        <v>4.7881498292179164E-30</v>
-      </c>
-      <c r="AH38">
-        <f t="shared" si="8"/>
-        <v>1.4705382716324417E-30</v>
-      </c>
-      <c r="AI38">
-        <f t="shared" si="8"/>
-        <v>4.6669946654011573E-31</v>
-      </c>
-      <c r="AJ38">
-        <f t="shared" si="8"/>
-        <v>1.527826213029459E-31</v>
-      </c>
-      <c r="AK38">
-        <f t="shared" si="8"/>
-        <v>5.15073568808805E-32</v>
-      </c>
-      <c r="AL38">
-        <f t="shared" si="8"/>
-        <v>1.7854996584394469E-32</v>
-      </c>
-      <c r="AM38">
-        <f t="shared" si="8"/>
-        <v>6.3552150923672423E-33</v>
-      </c>
-      <c r="AN38">
-        <f t="shared" si="8"/>
-        <v>2.3195783026428018E-33</v>
-      </c>
-      <c r="AO38">
-        <f t="shared" si="8"/>
-        <v>8.6708940399336025E-34</v>
-      </c>
-      <c r="AP38">
-        <f t="shared" si="8"/>
-        <v>3.3158763779250671E-34</v>
-      </c>
-      <c r="AQ38">
-        <f t="shared" si="8"/>
-        <v>1.2958314911791891E-34</v>
-      </c>
-      <c r="AR38">
-        <f t="shared" si="8"/>
-        <v>5.1698786237083942E-35</v>
-      </c>
-      <c r="AS38">
-        <f t="shared" si="8"/>
-        <v>2.1037147637148089E-35</v>
-      </c>
-      <c r="AT38">
-        <f t="shared" si="8"/>
-        <v>8.7234056883924656E-36</v>
-      </c>
-      <c r="AU38">
-        <f t="shared" si="8"/>
-        <v>3.6831460294800421E-36</v>
-      </c>
-      <c r="AV38">
-        <f t="shared" si="8"/>
-        <v>1.5821495221416938E-36</v>
-      </c>
-      <c r="AW38">
-        <f t="shared" si="8"/>
-        <v>6.9096077506499877E-37</v>
-      </c>
-      <c r="AX38">
-        <f t="shared" si="8"/>
-        <v>3.0657458533269204E-37</v>
-      </c>
-      <c r="AY38">
-        <f t="shared" si="8"/>
-        <v>1.3810586242954722E-37</v>
-      </c>
-      <c r="AZ38">
-        <f t="shared" si="8"/>
-        <v>6.312670744439288E-38</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>

</xml_diff>